<commit_message>
added MAE related files
</commit_message>
<xml_diff>
--- a/Optimization_analysis/my picks/feb_my_chosen_windows.xlsx
+++ b/Optimization_analysis/my picks/feb_my_chosen_windows.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vova deduskin lap\PycharmProjects\1500_count\Optimization_analysis\my picks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liikurserv\PycharmProjects\1500_count\Optimization_analysis\my picks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7474259C-8339-4050-9F0C-166F8F9A21F2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDE4B0B-ECF9-4C8C-9637-A7B482D04CE1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{B16AB54F-4DE5-4D0D-AB40-175C01783830}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>SourceFile</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>0630 0700.xlsx_all_month_specific_rows.xlsx</t>
-  </si>
-  <si>
-    <t>0700 0730.xlsx_all_month_specific_rows.xlsx</t>
   </si>
   <si>
     <t>0830 0900.xlsx_all_month_specific_rows.xlsx</t>
@@ -163,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +175,14 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -221,12 +226,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,15 +594,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453B8184-9089-4706-8AEA-41522E03988E}">
-  <dimension ref="A1:X21"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -607,7 +616,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -673,7 +682,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -681,7 +690,7 @@
       <c r="C2">
         <v>5145.5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>145.5</v>
       </c>
       <c r="E2">
@@ -755,7 +764,7 @@
       <c r="C3">
         <v>5141.5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>141.5</v>
       </c>
       <c r="E3">
@@ -829,7 +838,7 @@
       <c r="C4">
         <v>5251</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>251</v>
       </c>
       <c r="E4">
@@ -903,7 +912,7 @@
       <c r="C5">
         <v>5172</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>172</v>
       </c>
       <c r="E5">
@@ -977,7 +986,7 @@
       <c r="C6">
         <v>5293</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>293</v>
       </c>
       <c r="E6">
@@ -1051,7 +1060,7 @@
       <c r="C7">
         <v>5289</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>289</v>
       </c>
       <c r="E7">
@@ -1125,7 +1134,7 @@
       <c r="C8">
         <v>5192.5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>192.5</v>
       </c>
       <c r="E8">
@@ -1197,31 +1206,31 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>5184.5</v>
-      </c>
-      <c r="D9">
-        <v>184.5</v>
+        <v>5365</v>
+      </c>
+      <c r="D9" s="3">
+        <v>365</v>
       </c>
       <c r="E9">
-        <v>6.5892860000000004</v>
+        <v>20.277778000000001</v>
       </c>
       <c r="F9">
-        <v>1.453317</v>
+        <v>1.8924209999999999</v>
       </c>
       <c r="G9">
-        <v>1.4527559999999999</v>
+        <v>1.4092659999999999</v>
       </c>
       <c r="H9">
-        <v>8.3701699999999999</v>
+        <v>10.424122000000001</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>2.5228000000000002</v>
+        <v>4.6052999999999997</v>
       </c>
       <c r="K9">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L9" t="b">
         <v>0</v>
@@ -1271,28 +1280,28 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>5365</v>
-      </c>
-      <c r="D10">
-        <v>365</v>
+        <v>5352</v>
+      </c>
+      <c r="D10" s="3">
+        <v>352</v>
       </c>
       <c r="E10">
-        <v>20.277778000000001</v>
+        <v>19.555555999999999</v>
       </c>
       <c r="F10">
-        <v>1.8924209999999999</v>
+        <v>1.5966100000000001</v>
       </c>
       <c r="G10">
-        <v>1.4092659999999999</v>
+        <v>1.277677</v>
       </c>
       <c r="H10">
-        <v>10.424122000000001</v>
+        <v>6.4218070000000003</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>4.6052999999999997</v>
+        <v>5.4004000000000003</v>
       </c>
       <c r="K10">
         <v>18</v>
@@ -1345,31 +1354,31 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>5352</v>
-      </c>
-      <c r="D11">
-        <v>352</v>
+        <v>5355.5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>355.5</v>
       </c>
       <c r="E11">
-        <v>19.555555999999999</v>
+        <v>35.549999999999997</v>
       </c>
       <c r="F11">
-        <v>1.5966100000000001</v>
+        <v>1.9080459999999999</v>
       </c>
       <c r="G11">
-        <v>1.277677</v>
+        <v>0.82770699999999997</v>
       </c>
       <c r="H11">
-        <v>6.4218070000000003</v>
+        <v>2.0770369999999998</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>5.4004000000000003</v>
+        <v>7.8361999999999998</v>
       </c>
       <c r="K11">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="L11" t="b">
         <v>0</v>
@@ -1411,7 +1420,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1419,28 +1428,28 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>5355.5</v>
-      </c>
-      <c r="D12">
-        <v>355.5</v>
+        <v>5323.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>323.5</v>
       </c>
       <c r="E12">
-        <v>35.549999999999997</v>
+        <v>32.35</v>
       </c>
       <c r="F12">
-        <v>1.9080459999999999</v>
+        <v>2.6718350000000002</v>
       </c>
       <c r="G12">
-        <v>0.82770699999999997</v>
+        <v>2.262238</v>
       </c>
       <c r="H12">
-        <v>2.0770369999999998</v>
+        <v>3.3148900000000001</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
-        <v>7.8361999999999998</v>
+        <v>2.8319999999999999</v>
       </c>
       <c r="K12">
         <v>10</v>
@@ -1493,31 +1502,31 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>5323.5</v>
-      </c>
-      <c r="D13">
-        <v>323.5</v>
+        <v>5386.5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>386.5</v>
       </c>
       <c r="E13">
-        <v>32.35</v>
+        <v>42.944443999999997</v>
       </c>
       <c r="F13">
-        <v>2.6718350000000002</v>
+        <v>1.6692640000000001</v>
       </c>
       <c r="G13">
-        <v>2.262238</v>
+        <v>0.77532599999999996</v>
       </c>
       <c r="H13">
-        <v>3.3148900000000001</v>
+        <v>1.1979770000000001</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>2.8319999999999999</v>
+        <v>9.0496999999999996</v>
       </c>
       <c r="K13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L13" t="b">
         <v>0</v>
@@ -1567,31 +1576,31 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>5386.5</v>
-      </c>
-      <c r="D14">
-        <v>386.5</v>
+        <v>5448</v>
+      </c>
+      <c r="D14" s="3">
+        <v>448</v>
       </c>
       <c r="E14">
-        <v>42.944443999999997</v>
+        <v>26.352941000000001</v>
       </c>
       <c r="F14">
-        <v>1.6692640000000001</v>
+        <v>1.4906900000000001</v>
       </c>
       <c r="G14">
-        <v>0.77532599999999996</v>
+        <v>0.58295399999999997</v>
       </c>
       <c r="H14">
-        <v>1.1979770000000001</v>
+        <v>4.6847500000000002</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
-        <v>9.0496999999999996</v>
+        <v>13.3978</v>
       </c>
       <c r="K14">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L14" t="b">
         <v>0</v>
@@ -1633,7 +1642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1641,31 +1650,31 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>5448</v>
-      </c>
-      <c r="D15">
-        <v>448</v>
+        <v>5576.5</v>
+      </c>
+      <c r="D15" s="3">
+        <v>576.5</v>
       </c>
       <c r="E15">
-        <v>26.352941000000001</v>
+        <v>44.346153999999999</v>
       </c>
       <c r="F15">
-        <v>1.4906900000000001</v>
+        <v>1.90716</v>
       </c>
       <c r="G15">
-        <v>0.58295399999999997</v>
+        <v>1.874797</v>
       </c>
       <c r="H15">
-        <v>4.6847500000000002</v>
+        <v>5.9763919999999997</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>13.3978</v>
+        <v>5.226</v>
       </c>
       <c r="K15">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L15" t="b">
         <v>0</v>
@@ -1715,31 +1724,31 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>5576.5</v>
-      </c>
-      <c r="D16">
-        <v>576.5</v>
+        <v>5148.5</v>
+      </c>
+      <c r="D16" s="3">
+        <v>148.5</v>
       </c>
       <c r="E16">
-        <v>44.346153999999999</v>
+        <v>9.28125</v>
       </c>
       <c r="F16">
-        <v>1.90716</v>
+        <v>1.2314890000000001</v>
       </c>
       <c r="G16">
-        <v>1.874797</v>
+        <v>0.44594600000000001</v>
       </c>
       <c r="H16">
-        <v>5.9763919999999997</v>
+        <v>2.8858060000000001</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>5.226</v>
+        <v>6.1803999999999997</v>
       </c>
       <c r="K16">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L16" t="b">
         <v>0</v>
@@ -1789,28 +1798,28 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>5148.5</v>
-      </c>
-      <c r="D17">
-        <v>148.5</v>
+        <v>5605.5</v>
+      </c>
+      <c r="D17" s="3">
+        <v>605.5</v>
       </c>
       <c r="E17">
-        <v>9.28125</v>
+        <v>37.84375</v>
       </c>
       <c r="F17">
-        <v>1.2314890000000001</v>
+        <v>2.0176470000000002</v>
       </c>
       <c r="G17">
-        <v>0.44594600000000001</v>
+        <v>1.904088</v>
       </c>
       <c r="H17">
-        <v>2.8858060000000001</v>
+        <v>9.4992850000000004</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>6.1803999999999997</v>
+        <v>5.8173000000000004</v>
       </c>
       <c r="K17">
         <v>16</v>
@@ -1863,31 +1872,31 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>5605.5</v>
-      </c>
-      <c r="D18">
-        <v>605.5</v>
+        <v>5219</v>
+      </c>
+      <c r="D18" s="3">
+        <v>219</v>
       </c>
       <c r="E18">
-        <v>37.84375</v>
+        <v>27.375</v>
       </c>
       <c r="F18">
-        <v>2.0176470000000002</v>
+        <v>1.7807489999999999</v>
       </c>
       <c r="G18">
-        <v>1.904088</v>
+        <v>1.086849</v>
       </c>
       <c r="H18">
-        <v>9.4992850000000004</v>
+        <v>1.5005679999999999</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>5.8173000000000004</v>
+        <v>3.9641999999999999</v>
       </c>
       <c r="K18">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L18" t="b">
         <v>0</v>
@@ -1937,31 +1946,31 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>5219</v>
-      </c>
-      <c r="D19">
-        <v>219</v>
+        <v>5313.5</v>
+      </c>
+      <c r="D19" s="3">
+        <v>313.5</v>
       </c>
       <c r="E19">
-        <v>27.375</v>
+        <v>18.441175999999999</v>
       </c>
       <c r="F19">
-        <v>1.7807489999999999</v>
+        <v>1.7665040000000001</v>
       </c>
       <c r="G19">
-        <v>1.086849</v>
+        <v>1.026187</v>
       </c>
       <c r="H19">
-        <v>1.5005679999999999</v>
+        <v>9.7176849999999995</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
-        <v>3.9641999999999999</v>
+        <v>5.7674000000000003</v>
       </c>
       <c r="K19">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="L19" t="b">
         <v>0</v>
@@ -2011,31 +2020,31 @@
         <v>2</v>
       </c>
       <c r="C20">
-        <v>5313.5</v>
-      </c>
-      <c r="D20">
-        <v>313.5</v>
+        <v>5552.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>552.5</v>
       </c>
       <c r="E20">
-        <v>18.441175999999999</v>
+        <v>50.227272999999997</v>
       </c>
       <c r="F20">
-        <v>1.7665040000000001</v>
+        <v>4.2985069999999999</v>
       </c>
       <c r="G20">
-        <v>1.026187</v>
+        <v>2.5519630000000002</v>
       </c>
       <c r="H20">
-        <v>9.7176849999999995</v>
+        <v>1.7691460000000001</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>5.7674000000000003</v>
+        <v>4.1811999999999996</v>
       </c>
       <c r="K20">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="L20" t="b">
         <v>0</v>
@@ -2077,92 +2086,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>5552.5</v>
-      </c>
-      <c r="D21">
-        <v>552.5</v>
-      </c>
-      <c r="E21">
-        <v>50.227272999999997</v>
-      </c>
-      <c r="F21">
-        <v>4.2985069999999999</v>
-      </c>
-      <c r="G21">
-        <v>2.5519630000000002</v>
-      </c>
-      <c r="H21">
-        <v>1.7691460000000001</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>4.1811999999999996</v>
-      </c>
-      <c r="K21">
-        <v>11</v>
-      </c>
-      <c r="L21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" t="b">
-        <v>0</v>
-      </c>
-      <c r="O21" t="b">
-        <v>0</v>
-      </c>
-      <c r="P21" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q21" t="b">
-        <v>0</v>
-      </c>
-      <c r="R21" t="b">
-        <v>0</v>
-      </c>
-      <c r="S21" t="b">
-        <v>0</v>
-      </c>
-      <c r="T21" t="b">
-        <v>0</v>
-      </c>
-      <c r="U21" t="b">
-        <v>0</v>
-      </c>
-      <c r="V21" t="b">
-        <v>0</v>
-      </c>
-      <c r="W21" t="b">
-        <v>0</v>
-      </c>
-      <c r="X21" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:W1 L3:W21">
+  <conditionalFormatting sqref="L1:W1 L3:W20">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1 D3:D21">
+  <conditionalFormatting sqref="D1 D3:D20">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J21">
+  <conditionalFormatting sqref="J3:J20">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>10</formula>
     </cfRule>

</xml_diff>